<commit_message>
update folder to group
</commit_message>
<xml_diff>
--- a/smart-docs/docs/nstatic/files/smart-user-roles.xlsx
+++ b/smart-docs/docs/nstatic/files/smart-user-roles.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rchew/Documents/projects/smart/docs/smart_rtd/docs/nstatic/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckery/Documents/SMART/SMART/smart-docs/docs/nstatic/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64595F2-9775-4348-9871-0CAF020CC9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28240" tabRatio="500"/>
+    <workbookView xWindow="36180" yWindow="800" windowWidth="34560" windowHeight="19800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Label Data</t>
   </si>
@@ -35,9 +36,6 @@
     <t>Skip Data</t>
   </si>
   <si>
-    <t>History Table</t>
-  </si>
-  <si>
     <t>Fix Skew</t>
   </si>
   <si>
@@ -93,13 +91,19 @@
   </si>
   <si>
     <t>✓</t>
+  </si>
+  <si>
+    <t>History Table (all labels)</t>
+  </si>
+  <si>
+    <t>History Table (my labels)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -410,74 +414,74 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,6 +492,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -755,14 +762,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="218" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
@@ -771,188 +778,198 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="2:5" ht="17" thickBot="1"/>
+    <row r="2" spans="2:5" ht="17" thickBot="1">
+      <c r="B2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="27" t="s">
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="24"/>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="24"/>
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="24"/>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="24"/>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="24"/>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="24"/>
+      <c r="C9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="2:5" ht="17" thickBot="1">
+      <c r="B10" s="25"/>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="24"/>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="2:5" ht="17" thickBot="1">
+      <c r="B13" s="26"/>
+      <c r="C13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="17" thickBot="1">
+      <c r="B15" s="25"/>
+      <c r="C15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="D16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="2:5" ht="17" thickBot="1">
+      <c r="B17" s="25"/>
+      <c r="C17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
+      <c r="D17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>